<commit_message>
changing AdvancedNuclear back to ConventionalNuclear in all files and tabs
</commit_message>
<xml_diff>
--- a/inputs/ALEAF_inputs/ALEAF_Master_LC_GEP_IL_C2N.xlsx
+++ b/inputs/ALEAF_inputs/ALEAF_Master_LC_GEP_IL_C2N.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\biegelk\abce\inputs\ALEAF_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF40D454-8BB9-468D-B3CA-5AA286736072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB88362-3300-495B-B1B1-3BA0A6DCCE7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" tabRatio="927" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" tabRatio="927" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LC_GEP Setting" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="309">
   <si>
     <t>Setting</t>
   </si>
@@ -481,9 +481,6 @@
   </si>
   <si>
     <t>Nuclear</t>
-  </si>
-  <si>
-    <t>AdvancedNuclear</t>
   </si>
   <si>
     <t>data_path</t>
@@ -2346,87 +2343,87 @@
   <sheetData>
     <row r="1" spans="1:26">
       <c r="A1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D1" t="s">
         <v>61</v>
       </c>
       <c r="E1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F1" t="s">
         <v>173</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
+        <v>169</v>
+      </c>
+      <c r="I1" t="s">
+        <v>206</v>
+      </c>
+      <c r="J1" t="s">
+        <v>207</v>
+      </c>
+      <c r="K1" t="s">
+        <v>208</v>
+      </c>
+      <c r="L1" t="s">
+        <v>209</v>
+      </c>
+      <c r="M1" t="s">
+        <v>210</v>
+      </c>
+      <c r="N1" t="s">
+        <v>211</v>
+      </c>
+      <c r="O1" t="s">
+        <v>212</v>
+      </c>
+      <c r="P1" t="s">
         <v>174</v>
       </c>
-      <c r="H1" t="s">
-        <v>170</v>
-      </c>
-      <c r="I1" t="s">
-        <v>207</v>
-      </c>
-      <c r="J1" t="s">
-        <v>208</v>
-      </c>
-      <c r="K1" t="s">
-        <v>209</v>
-      </c>
-      <c r="L1" t="s">
-        <v>210</v>
-      </c>
-      <c r="M1" t="s">
-        <v>211</v>
-      </c>
-      <c r="N1" t="s">
-        <v>212</v>
-      </c>
-      <c r="O1" t="s">
-        <v>213</v>
-      </c>
-      <c r="P1" t="s">
-        <v>175</v>
-      </c>
       <c r="Q1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="R1" t="s">
         <v>136</v>
       </c>
       <c r="S1" t="s">
+        <v>213</v>
+      </c>
+      <c r="T1" t="s">
         <v>214</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
+        <v>178</v>
+      </c>
+      <c r="X1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>169</v>
+      </c>
+      <c r="Z1" t="s">
         <v>215</v>
-      </c>
-      <c r="U1" t="s">
-        <v>179</v>
-      </c>
-      <c r="X1" t="s">
-        <v>169</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>170</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="2" spans="1:26">
       <c r="A2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C2" t="s">
         <v>93</v>
       </c>
       <c r="D2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E2">
         <v>2018</v>
@@ -2435,49 +2432,49 @@
         <v>2020</v>
       </c>
       <c r="I2" s="29" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="L2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="M2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="O2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="P2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Q2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="R2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="S2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="T2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="U2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="X2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="Y2" s="29" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="Z2">
         <v>15</v>
@@ -2485,64 +2482,64 @@
     </row>
     <row r="3" spans="1:26">
       <c r="A3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B3" t="s">
+        <v>218</v>
+      </c>
+      <c r="C3" t="s">
         <v>219</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>220</v>
-      </c>
-      <c r="D3" t="s">
-        <v>221</v>
       </c>
       <c r="E3">
         <v>2019</v>
       </c>
       <c r="I3" s="29" t="s">
+        <v>221</v>
+      </c>
+      <c r="J3" t="s">
         <v>222</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>223</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>224</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>225</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>226</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>227</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>228</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
+        <v>181</v>
+      </c>
+      <c r="R3">
+        <v>20</v>
+      </c>
+      <c r="S3" t="s">
         <v>229</v>
       </c>
-      <c r="Q3" t="s">
-        <v>182</v>
-      </c>
-      <c r="R3">
-        <v>20</v>
-      </c>
-      <c r="S3" t="s">
-        <v>230</v>
-      </c>
       <c r="T3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="U3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="X3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="Y3" s="29" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="Z3">
         <v>20</v>
@@ -2550,13 +2547,13 @@
     </row>
     <row r="4" spans="1:26">
       <c r="A4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E4">
         <v>2020</v>
@@ -2565,46 +2562,46 @@
         <v>15</v>
       </c>
       <c r="J4" t="s">
+        <v>231</v>
+      </c>
+      <c r="K4" t="s">
         <v>232</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>233</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>234</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>235</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>236</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>237</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>238</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4">
+        <v>30</v>
+      </c>
+      <c r="S4" t="s">
         <v>239</v>
       </c>
-      <c r="R4">
-        <v>30</v>
-      </c>
-      <c r="S4" t="s">
-        <v>240</v>
-      </c>
       <c r="T4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="U4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="X4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="Y4" s="29" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="Z4">
         <v>30</v>
@@ -2612,7 +2609,7 @@
     </row>
     <row r="5" spans="1:26">
       <c r="A5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E5">
         <v>2021</v>
@@ -2621,46 +2618,46 @@
         <v>20</v>
       </c>
       <c r="J5" t="s">
+        <v>240</v>
+      </c>
+      <c r="K5" t="s">
         <v>241</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>242</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>243</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>244</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>245</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>246</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>247</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>248</v>
       </c>
       <c r="R5">
         <v>60</v>
       </c>
       <c r="S5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="T5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="X5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="Y5" s="29" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="Z5">
         <v>15</v>
@@ -2668,7 +2665,7 @@
     </row>
     <row r="6" spans="1:26">
       <c r="A6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E6">
         <v>2022</v>
@@ -2680,40 +2677,40 @@
         <v>20</v>
       </c>
       <c r="K6" t="s">
+        <v>249</v>
+      </c>
+      <c r="L6" t="s">
+        <v>179</v>
+      </c>
+      <c r="M6">
+        <v>20</v>
+      </c>
+      <c r="N6" t="s">
         <v>250</v>
       </c>
-      <c r="L6" t="s">
-        <v>180</v>
-      </c>
-      <c r="M6">
-        <v>20</v>
-      </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>251</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>252</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>253</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="S6" t="s">
         <v>254</v>
       </c>
-      <c r="S6" t="s">
-        <v>255</v>
-      </c>
       <c r="T6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="U6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="X6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="Y6" s="29" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="Z6">
         <v>20</v>
@@ -2721,7 +2718,7 @@
     </row>
     <row r="7" spans="1:26">
       <c r="A7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E7">
         <v>2023</v>
@@ -2730,40 +2727,40 @@
         <v>30</v>
       </c>
       <c r="K7" t="s">
+        <v>255</v>
+      </c>
+      <c r="L7" t="s">
         <v>256</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7">
+        <v>30</v>
+      </c>
+      <c r="N7" t="s">
         <v>257</v>
       </c>
-      <c r="M7">
-        <v>30</v>
-      </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>258</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>182</v>
+      </c>
+      <c r="S7" t="s">
         <v>259</v>
       </c>
-      <c r="P7" t="s">
-        <v>176</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>183</v>
-      </c>
-      <c r="S7" t="s">
-        <v>260</v>
-      </c>
       <c r="T7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="U7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="X7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="Y7" s="29" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="Z7">
         <v>30</v>
@@ -2771,7 +2768,7 @@
     </row>
     <row r="8" spans="1:26">
       <c r="A8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E8">
         <v>2024</v>
@@ -2780,26 +2777,26 @@
         <v>45</v>
       </c>
       <c r="K8" t="s">
+        <v>260</v>
+      </c>
+      <c r="L8">
+        <v>20</v>
+      </c>
+      <c r="N8" t="s">
         <v>261</v>
       </c>
-      <c r="L8">
-        <v>20</v>
-      </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>262</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>263</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>264</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="S8" t="s">
         <v>265</v>
       </c>
-      <c r="S8" t="s">
-        <v>266</v>
-      </c>
       <c r="T8">
         <v>20</v>
       </c>
@@ -2807,10 +2804,10 @@
         <v>20</v>
       </c>
       <c r="X8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Y8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Z8">
         <v>20</v>
@@ -2818,32 +2815,32 @@
     </row>
     <row r="9" spans="1:26">
       <c r="A9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E9">
         <v>2025</v>
       </c>
       <c r="K9" t="s">
+        <v>266</v>
+      </c>
+      <c r="L9">
+        <v>30</v>
+      </c>
+      <c r="N9">
+        <v>20</v>
+      </c>
+      <c r="O9" t="s">
         <v>267</v>
       </c>
-      <c r="L9">
-        <v>30</v>
-      </c>
-      <c r="N9">
-        <v>20</v>
-      </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>268</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9">
+        <v>20</v>
+      </c>
+      <c r="S9" t="s">
         <v>269</v>
       </c>
-      <c r="Q9">
-        <v>20</v>
-      </c>
-      <c r="S9" t="s">
-        <v>270</v>
-      </c>
       <c r="T9">
         <v>30</v>
       </c>
@@ -2851,10 +2848,10 @@
         <v>30</v>
       </c>
       <c r="X9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Y9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Z9">
         <v>30</v>
@@ -2862,34 +2859,34 @@
     </row>
     <row r="10" spans="1:26">
       <c r="A10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E10">
         <v>2026</v>
       </c>
       <c r="K10" t="s">
+        <v>270</v>
+      </c>
+      <c r="N10">
+        <v>30</v>
+      </c>
+      <c r="O10" t="s">
         <v>271</v>
       </c>
-      <c r="N10">
-        <v>30</v>
-      </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
         <v>272</v>
       </c>
-      <c r="P10" t="s">
+      <c r="Q10">
+        <v>30</v>
+      </c>
+      <c r="S10" t="s">
         <v>273</v>
       </c>
-      <c r="Q10">
-        <v>30</v>
-      </c>
-      <c r="S10" t="s">
-        <v>274</v>
-      </c>
       <c r="X10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Y10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Z10">
         <v>45</v>
@@ -2909,19 +2906,19 @@
         <v>20</v>
       </c>
       <c r="P11" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="Q11">
         <v>55</v>
       </c>
       <c r="S11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="X11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Y11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Z11">
         <v>20</v>
@@ -2929,7 +2926,7 @@
     </row>
     <row r="12" spans="1:26">
       <c r="A12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E12">
         <v>2028</v>
@@ -2941,16 +2938,16 @@
         <v>30</v>
       </c>
       <c r="P12" t="s">
+        <v>276</v>
+      </c>
+      <c r="S12" t="s">
         <v>277</v>
       </c>
-      <c r="S12" t="s">
-        <v>278</v>
-      </c>
       <c r="X12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Y12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Z12">
         <v>30</v>
@@ -2958,7 +2955,7 @@
     </row>
     <row r="13" spans="1:26">
       <c r="A13" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E13">
         <v>2029</v>
@@ -2973,13 +2970,13 @@
         <v>20</v>
       </c>
       <c r="S13" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="X13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Y13" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Z13">
         <v>45</v>
@@ -2987,7 +2984,7 @@
     </row>
     <row r="14" spans="1:26">
       <c r="A14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E14">
         <v>2030</v>
@@ -2996,13 +2993,13 @@
         <v>30</v>
       </c>
       <c r="S14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="X14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Y14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="Z14">
         <v>20</v>
@@ -3013,13 +3010,13 @@
         <v>2031</v>
       </c>
       <c r="S15" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="X15" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Y15" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="Z15">
         <v>30</v>
@@ -3030,13 +3027,13 @@
         <v>2032</v>
       </c>
       <c r="S16" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="X16" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Y16" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="Z16">
         <v>45</v>
@@ -3050,10 +3047,10 @@
         <v>20</v>
       </c>
       <c r="X17" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Y17" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="Z17">
         <v>20</v>
@@ -3067,10 +3064,10 @@
         <v>30</v>
       </c>
       <c r="X18" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Y18" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="Z18">
         <v>30</v>
@@ -3081,10 +3078,10 @@
         <v>2035</v>
       </c>
       <c r="X19" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Y19" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="Z19">
         <v>45</v>
@@ -3095,10 +3092,10 @@
         <v>2036</v>
       </c>
       <c r="X20" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Y20" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Z20">
         <v>20</v>
@@ -3109,10 +3106,10 @@
         <v>2037</v>
       </c>
       <c r="X21" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Y21" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Z21">
         <v>30</v>
@@ -3123,10 +3120,10 @@
         <v>2038</v>
       </c>
       <c r="X22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Y22" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Z22">
         <v>75</v>
@@ -3137,10 +3134,10 @@
         <v>2039</v>
       </c>
       <c r="X23" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Y23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Z23">
         <v>20</v>
@@ -3151,10 +3148,10 @@
         <v>2040</v>
       </c>
       <c r="X24" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Y24" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Z24">
         <v>30</v>
@@ -3165,10 +3162,10 @@
         <v>2041</v>
       </c>
       <c r="X25" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Y25" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Z25">
         <v>75</v>
@@ -3179,10 +3176,10 @@
         <v>2042</v>
       </c>
       <c r="X26" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Y26" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="Z26">
         <v>20</v>
@@ -3193,10 +3190,10 @@
         <v>2043</v>
       </c>
       <c r="X27" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Y27" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="Z27">
         <v>30</v>
@@ -3207,10 +3204,10 @@
         <v>2044</v>
       </c>
       <c r="X28" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Y28" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="Z28">
         <v>75</v>
@@ -3221,10 +3218,10 @@
         <v>2045</v>
       </c>
       <c r="X29" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Y29" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="Z29">
         <v>20</v>
@@ -3235,10 +3232,10 @@
         <v>2046</v>
       </c>
       <c r="X30" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Y30" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="Z30">
         <v>30</v>
@@ -3249,10 +3246,10 @@
         <v>2047</v>
       </c>
       <c r="X31" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Y31" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="Z31">
         <v>75</v>
@@ -3263,10 +3260,10 @@
         <v>2048</v>
       </c>
       <c r="X32" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Y32" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="Z32">
         <v>20</v>
@@ -3277,10 +3274,10 @@
         <v>2049</v>
       </c>
       <c r="X33" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Y33" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="Z33">
         <v>30</v>
@@ -3291,10 +3288,10 @@
         <v>2050</v>
       </c>
       <c r="X34" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Y34" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="Z34">
         <v>75</v>
@@ -3302,10 +3299,10 @@
     </row>
     <row r="35" spans="5:26">
       <c r="X35" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Y35" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="Z35">
         <v>20</v>
@@ -3313,10 +3310,10 @@
     </row>
     <row r="36" spans="5:26">
       <c r="X36" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Y36" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="Z36">
         <v>30</v>
@@ -3324,10 +3321,10 @@
     </row>
     <row r="37" spans="5:26">
       <c r="X37" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Y37" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="Z37">
         <v>75</v>
@@ -3335,10 +3332,10 @@
     </row>
     <row r="38" spans="5:26">
       <c r="X38" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Y38" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="Z38">
         <v>20</v>
@@ -3346,10 +3343,10 @@
     </row>
     <row r="39" spans="5:26">
       <c r="X39" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Y39" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="Z39">
         <v>30</v>
@@ -3357,10 +3354,10 @@
     </row>
     <row r="40" spans="5:26">
       <c r="X40" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Y40" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="Z40">
         <v>75</v>
@@ -3368,10 +3365,10 @@
     </row>
     <row r="41" spans="5:26">
       <c r="X41" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Y41" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="Z41">
         <v>20</v>
@@ -3379,10 +3376,10 @@
     </row>
     <row r="42" spans="5:26">
       <c r="X42" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Y42" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="Z42">
         <v>30</v>
@@ -3390,10 +3387,10 @@
     </row>
     <row r="43" spans="5:26">
       <c r="X43" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Y43" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="Z43">
         <v>75</v>
@@ -3401,10 +3398,10 @@
     </row>
     <row r="44" spans="5:26">
       <c r="X44" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Y44" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="Z44">
         <v>20</v>
@@ -3412,10 +3409,10 @@
     </row>
     <row r="45" spans="5:26">
       <c r="X45" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Y45" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="Z45">
         <v>30</v>
@@ -3423,10 +3420,10 @@
     </row>
     <row r="46" spans="5:26">
       <c r="X46" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Y46" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="Z46">
         <v>75</v>
@@ -3434,10 +3431,10 @@
     </row>
     <row r="47" spans="5:26">
       <c r="X47" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="Y47" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Z47">
         <v>20</v>
@@ -3445,10 +3442,10 @@
     </row>
     <row r="48" spans="5:26">
       <c r="X48" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="Y48" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Z48">
         <v>30</v>
@@ -3456,10 +3453,10 @@
     </row>
     <row r="49" spans="24:26">
       <c r="X49" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="Y49" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="Z49">
         <v>20</v>
@@ -3467,10 +3464,10 @@
     </row>
     <row r="50" spans="24:26">
       <c r="X50" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="Y50" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="Z50">
         <v>30</v>
@@ -3478,10 +3475,10 @@
     </row>
     <row r="51" spans="24:26">
       <c r="X51" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="Y51" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Z51">
         <v>20</v>
@@ -3489,10 +3486,10 @@
     </row>
     <row r="52" spans="24:26">
       <c r="X52" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="Y52" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Z52">
         <v>30</v>
@@ -3500,10 +3497,10 @@
     </row>
     <row r="53" spans="24:26">
       <c r="X53" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="Y53" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="Z53">
         <v>20</v>
@@ -3511,10 +3508,10 @@
     </row>
     <row r="54" spans="24:26">
       <c r="X54" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="Y54" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="Z54">
         <v>30</v>
@@ -3522,10 +3519,10 @@
     </row>
     <row r="55" spans="24:26">
       <c r="X55" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="Y55" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="Z55">
         <v>20</v>
@@ -3533,10 +3530,10 @@
     </row>
     <row r="56" spans="24:26">
       <c r="X56" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="Y56" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="Z56">
         <v>30</v>
@@ -3544,10 +3541,10 @@
     </row>
     <row r="57" spans="24:26">
       <c r="X57" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="Y57" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="Z57">
         <v>20</v>
@@ -3555,10 +3552,10 @@
     </row>
     <row r="58" spans="24:26">
       <c r="X58" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="Y58" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="Z58">
         <v>30</v>
@@ -3566,10 +3563,10 @@
     </row>
     <row r="59" spans="24:26">
       <c r="X59" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="Y59" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Z59">
         <v>20</v>
@@ -3577,10 +3574,10 @@
     </row>
     <row r="60" spans="24:26">
       <c r="X60" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="Y60" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Z60">
         <v>30</v>
@@ -3588,10 +3585,10 @@
     </row>
     <row r="61" spans="24:26">
       <c r="X61" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="Y61" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="Z61">
         <v>20</v>
@@ -3599,10 +3596,10 @@
     </row>
     <row r="62" spans="24:26">
       <c r="X62" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="Y62" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="Z62">
         <v>30</v>
@@ -3610,10 +3607,10 @@
     </row>
     <row r="63" spans="24:26">
       <c r="X63" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="Y63" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Z63">
         <v>20</v>
@@ -3621,10 +3618,10 @@
     </row>
     <row r="64" spans="24:26">
       <c r="X64" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="Y64" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Z64">
         <v>30</v>
@@ -3632,10 +3629,10 @@
     </row>
     <row r="65" spans="24:26">
       <c r="X65" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="Y65" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="Z65">
         <v>20</v>
@@ -3643,10 +3640,10 @@
     </row>
     <row r="66" spans="24:26">
       <c r="X66" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="Y66" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="Z66">
         <v>30</v>
@@ -3654,10 +3651,10 @@
     </row>
     <row r="67" spans="24:26">
       <c r="X67" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="Y67" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Z67">
         <v>20</v>
@@ -3665,10 +3662,10 @@
     </row>
     <row r="68" spans="24:26">
       <c r="X68" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="Y68" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Z68">
         <v>30</v>
@@ -3676,10 +3673,10 @@
     </row>
     <row r="69" spans="24:26">
       <c r="X69" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="Y69" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="Z69">
         <v>20</v>
@@ -3687,10 +3684,10 @@
     </row>
     <row r="70" spans="24:26">
       <c r="X70" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="Y70" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="Z70">
         <v>30</v>
@@ -3698,10 +3695,10 @@
     </row>
     <row r="71" spans="24:26">
       <c r="X71" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="Y71" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Z71">
         <v>20</v>
@@ -3709,10 +3706,10 @@
     </row>
     <row r="72" spans="24:26">
       <c r="X72" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="Y72" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Z72">
         <v>30</v>
@@ -3720,10 +3717,10 @@
     </row>
     <row r="73" spans="24:26">
       <c r="X73" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="Y73" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="Z73">
         <v>20</v>
@@ -3731,10 +3728,10 @@
     </row>
     <row r="74" spans="24:26">
       <c r="X74" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="Y74" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="Z74">
         <v>30</v>
@@ -3742,10 +3739,10 @@
     </row>
     <row r="75" spans="24:26">
       <c r="X75" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="Y75" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="Z75">
         <v>20</v>
@@ -3753,10 +3750,10 @@
     </row>
     <row r="76" spans="24:26">
       <c r="X76" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="Y76" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="Z76">
         <v>30</v>
@@ -3764,10 +3761,10 @@
     </row>
     <row r="77" spans="24:26">
       <c r="X77" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="Y77" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="Z77">
         <v>20</v>
@@ -3775,10 +3772,10 @@
     </row>
     <row r="78" spans="24:26">
       <c r="X78" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="Y78" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="Z78">
         <v>30</v>
@@ -3786,10 +3783,10 @@
     </row>
     <row r="79" spans="24:26">
       <c r="X79" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="Y79" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Z79">
         <v>20</v>
@@ -3797,10 +3794,10 @@
     </row>
     <row r="80" spans="24:26">
       <c r="X80" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="Y80" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Z80">
         <v>30</v>
@@ -3808,10 +3805,10 @@
     </row>
     <row r="81" spans="24:26">
       <c r="X81" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Y81" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Z81">
         <v>20</v>
@@ -3819,10 +3816,10 @@
     </row>
     <row r="82" spans="24:26">
       <c r="X82" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Y82" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Z82">
         <v>30</v>
@@ -3830,10 +3827,10 @@
     </row>
     <row r="83" spans="24:26">
       <c r="X83" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Y83" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Z83">
         <v>100</v>
@@ -3841,10 +3838,10 @@
     </row>
     <row r="84" spans="24:26">
       <c r="X84" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Y84" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="Z84">
         <v>20</v>
@@ -3852,10 +3849,10 @@
     </row>
     <row r="85" spans="24:26">
       <c r="X85" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Y85" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="Z85">
         <v>30</v>
@@ -3863,10 +3860,10 @@
     </row>
     <row r="86" spans="24:26">
       <c r="X86" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Y86" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="Z86">
         <v>100</v>
@@ -3874,10 +3871,10 @@
     </row>
     <row r="87" spans="24:26">
       <c r="X87" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Y87" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Z87">
         <v>20</v>
@@ -3885,10 +3882,10 @@
     </row>
     <row r="88" spans="24:26">
       <c r="X88" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Y88" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Z88">
         <v>30</v>
@@ -3896,10 +3893,10 @@
     </row>
     <row r="89" spans="24:26">
       <c r="X89" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Y89" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Z89">
         <v>100</v>
@@ -3907,10 +3904,10 @@
     </row>
     <row r="90" spans="24:26">
       <c r="X90" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Y90" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Z90">
         <v>20</v>
@@ -3918,10 +3915,10 @@
     </row>
     <row r="91" spans="24:26">
       <c r="X91" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Y91" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Z91">
         <v>30</v>
@@ -3929,10 +3926,10 @@
     </row>
     <row r="92" spans="24:26">
       <c r="X92" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Y92" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Z92">
         <v>100</v>
@@ -3940,10 +3937,10 @@
     </row>
     <row r="93" spans="24:26">
       <c r="X93" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Y93" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="Z93">
         <v>20</v>
@@ -3951,10 +3948,10 @@
     </row>
     <row r="94" spans="24:26">
       <c r="X94" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Y94" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="Z94">
         <v>30</v>
@@ -3962,10 +3959,10 @@
     </row>
     <row r="95" spans="24:26">
       <c r="X95" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Y95" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="Z95">
         <v>100</v>
@@ -3973,10 +3970,10 @@
     </row>
     <row r="96" spans="24:26">
       <c r="X96" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Y96" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="Z96">
         <v>20</v>
@@ -3984,10 +3981,10 @@
     </row>
     <row r="97" spans="24:26">
       <c r="X97" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Y97" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="Z97">
         <v>30</v>
@@ -3995,10 +3992,10 @@
     </row>
     <row r="98" spans="24:26">
       <c r="X98" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Y98" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="Z98">
         <v>100</v>
@@ -4006,10 +4003,10 @@
     </row>
     <row r="99" spans="24:26">
       <c r="X99" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Y99" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="Z99">
         <v>20</v>
@@ -4017,10 +4014,10 @@
     </row>
     <row r="100" spans="24:26">
       <c r="X100" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Y100" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="Z100">
         <v>30</v>
@@ -4028,10 +4025,10 @@
     </row>
     <row r="101" spans="24:26">
       <c r="X101" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Y101" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="Z101">
         <v>100</v>
@@ -4039,10 +4036,10 @@
     </row>
     <row r="102" spans="24:26">
       <c r="X102" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Y102" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Z102">
         <v>20</v>
@@ -4050,10 +4047,10 @@
     </row>
     <row r="103" spans="24:26">
       <c r="X103" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Y103" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Z103">
         <v>30</v>
@@ -4061,10 +4058,10 @@
     </row>
     <row r="104" spans="24:26">
       <c r="X104" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Y104" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Z104">
         <v>100</v>
@@ -4072,10 +4069,10 @@
     </row>
     <row r="105" spans="24:26">
       <c r="X105" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Y105" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="Z105">
         <v>20</v>
@@ -4083,10 +4080,10 @@
     </row>
     <row r="106" spans="24:26">
       <c r="X106" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Y106" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="Z106">
         <v>30</v>
@@ -4094,10 +4091,10 @@
     </row>
     <row r="107" spans="24:26">
       <c r="X107" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Y107" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="Z107">
         <v>100</v>
@@ -4105,10 +4102,10 @@
     </row>
     <row r="108" spans="24:26">
       <c r="X108" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="Y108" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Z108">
         <v>20</v>
@@ -4116,10 +4113,10 @@
     </row>
     <row r="109" spans="24:26">
       <c r="X109" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="Y109" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Z109">
         <v>30</v>
@@ -4127,10 +4124,10 @@
     </row>
     <row r="110" spans="24:26">
       <c r="X110" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="Y110" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="Z110">
         <v>20</v>
@@ -4138,10 +4135,10 @@
     </row>
     <row r="111" spans="24:26">
       <c r="X111" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="Y111" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="Z111">
         <v>30</v>
@@ -4149,10 +4146,10 @@
     </row>
     <row r="112" spans="24:26">
       <c r="X112" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="Y112" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="Z112">
         <v>20</v>
@@ -4160,10 +4157,10 @@
     </row>
     <row r="113" spans="24:26">
       <c r="X113" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="Y113" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="Z113">
         <v>30</v>
@@ -4171,10 +4168,10 @@
     </row>
     <row r="114" spans="24:26">
       <c r="X114" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="Y114" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Z114">
         <v>20</v>
@@ -4182,10 +4179,10 @@
     </row>
     <row r="115" spans="24:26">
       <c r="X115" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="Y115" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Z115">
         <v>30</v>
@@ -4193,10 +4190,10 @@
     </row>
     <row r="116" spans="24:26">
       <c r="X116" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="Y116" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Z116">
         <v>20</v>
@@ -4204,10 +4201,10 @@
     </row>
     <row r="117" spans="24:26">
       <c r="X117" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="Y117" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Z117">
         <v>30</v>
@@ -4215,10 +4212,10 @@
     </row>
     <row r="118" spans="24:26">
       <c r="X118" t="s">
+        <v>174</v>
+      </c>
+      <c r="Y118" t="s">
         <v>175</v>
-      </c>
-      <c r="Y118" t="s">
-        <v>176</v>
       </c>
       <c r="Z118">
         <v>20</v>
@@ -4226,10 +4223,10 @@
     </row>
     <row r="119" spans="24:26">
       <c r="X119" t="s">
+        <v>174</v>
+      </c>
+      <c r="Y119" t="s">
         <v>175</v>
-      </c>
-      <c r="Y119" t="s">
-        <v>176</v>
       </c>
       <c r="Z119">
         <v>30</v>
@@ -4237,10 +4234,10 @@
     </row>
     <row r="120" spans="24:26">
       <c r="X120" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="Y120" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="Z120">
         <v>20</v>
@@ -4248,10 +4245,10 @@
     </row>
     <row r="121" spans="24:26">
       <c r="X121" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="Y121" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="Z121">
         <v>30</v>
@@ -4259,10 +4256,10 @@
     </row>
     <row r="122" spans="24:26">
       <c r="X122" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="Y122" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="Z122">
         <v>20</v>
@@ -4270,10 +4267,10 @@
     </row>
     <row r="123" spans="24:26">
       <c r="X123" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="Y123" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="Z123">
         <v>30</v>
@@ -4281,10 +4278,10 @@
     </row>
     <row r="124" spans="24:26">
       <c r="X124" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="Y124" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="Z124">
         <v>20</v>
@@ -4292,10 +4289,10 @@
     </row>
     <row r="125" spans="24:26">
       <c r="X125" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="Y125" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="Z125">
         <v>30</v>
@@ -4303,10 +4300,10 @@
     </row>
     <row r="126" spans="24:26">
       <c r="X126" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="Y126" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="Z126">
         <v>20</v>
@@ -4314,10 +4311,10 @@
     </row>
     <row r="127" spans="24:26">
       <c r="X127" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="Y127" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="Z127">
         <v>30</v>
@@ -4325,10 +4322,10 @@
     </row>
     <row r="128" spans="24:26">
       <c r="X128" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="Y128" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="Z128">
         <v>20</v>
@@ -4336,10 +4333,10 @@
     </row>
     <row r="129" spans="24:26">
       <c r="X129" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="Y129" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="Z129">
         <v>30</v>
@@ -4347,10 +4344,10 @@
     </row>
     <row r="130" spans="24:26">
       <c r="X130" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Y130" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Z130">
         <v>20</v>
@@ -4358,10 +4355,10 @@
     </row>
     <row r="131" spans="24:26">
       <c r="X131" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Y131" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Z131">
         <v>30</v>
@@ -4369,10 +4366,10 @@
     </row>
     <row r="132" spans="24:26">
       <c r="X132" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Y132" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Z132">
         <v>55</v>
@@ -4380,10 +4377,10 @@
     </row>
     <row r="133" spans="24:26">
       <c r="X133" t="s">
+        <v>180</v>
+      </c>
+      <c r="Y133" t="s">
         <v>181</v>
-      </c>
-      <c r="Y133" t="s">
-        <v>182</v>
       </c>
       <c r="Z133">
         <v>20</v>
@@ -4391,10 +4388,10 @@
     </row>
     <row r="134" spans="24:26">
       <c r="X134" t="s">
+        <v>180</v>
+      </c>
+      <c r="Y134" t="s">
         <v>181</v>
-      </c>
-      <c r="Y134" t="s">
-        <v>182</v>
       </c>
       <c r="Z134">
         <v>30</v>
@@ -4402,10 +4399,10 @@
     </row>
     <row r="135" spans="24:26">
       <c r="X135" t="s">
+        <v>180</v>
+      </c>
+      <c r="Y135" t="s">
         <v>181</v>
-      </c>
-      <c r="Y135" t="s">
-        <v>182</v>
       </c>
       <c r="Z135">
         <v>55</v>
@@ -4413,10 +4410,10 @@
     </row>
     <row r="136" spans="24:26">
       <c r="X136" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Y136" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="Z136">
         <v>20</v>
@@ -4424,10 +4421,10 @@
     </row>
     <row r="137" spans="24:26">
       <c r="X137" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Y137" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="Z137">
         <v>30</v>
@@ -4435,10 +4432,10 @@
     </row>
     <row r="138" spans="24:26">
       <c r="X138" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Y138" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="Z138">
         <v>55</v>
@@ -4446,10 +4443,10 @@
     </row>
     <row r="139" spans="24:26">
       <c r="X139" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Y139" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="Z139">
         <v>20</v>
@@ -4457,10 +4454,10 @@
     </row>
     <row r="140" spans="24:26">
       <c r="X140" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Y140" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="Z140">
         <v>30</v>
@@ -4468,10 +4465,10 @@
     </row>
     <row r="141" spans="24:26">
       <c r="X141" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Y141" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="Z141">
         <v>55</v>
@@ -4479,10 +4476,10 @@
     </row>
     <row r="142" spans="24:26">
       <c r="X142" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Y142" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="Z142">
         <v>20</v>
@@ -4490,10 +4487,10 @@
     </row>
     <row r="143" spans="24:26">
       <c r="X143" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Y143" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="Z143">
         <v>30</v>
@@ -4501,10 +4498,10 @@
     </row>
     <row r="144" spans="24:26">
       <c r="X144" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Y144" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="Z144">
         <v>55</v>
@@ -4512,10 +4509,10 @@
     </row>
     <row r="145" spans="24:26">
       <c r="X145" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Y145" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="Z145">
         <v>20</v>
@@ -4523,10 +4520,10 @@
     </row>
     <row r="146" spans="24:26">
       <c r="X146" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Y146" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="Z146">
         <v>30</v>
@@ -4534,10 +4531,10 @@
     </row>
     <row r="147" spans="24:26">
       <c r="X147" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Y147" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="Z147">
         <v>55</v>
@@ -4545,10 +4542,10 @@
     </row>
     <row r="148" spans="24:26">
       <c r="X148" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Y148" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="Z148">
         <v>20</v>
@@ -4556,10 +4553,10 @@
     </row>
     <row r="149" spans="24:26">
       <c r="X149" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Y149" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="Z149">
         <v>30</v>
@@ -4567,10 +4564,10 @@
     </row>
     <row r="150" spans="24:26">
       <c r="X150" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Y150" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="Z150">
         <v>55</v>
@@ -4581,7 +4578,7 @@
         <v>136</v>
       </c>
       <c r="Y151" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Z151">
         <v>20</v>
@@ -4592,7 +4589,7 @@
         <v>136</v>
       </c>
       <c r="Y152" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Z152">
         <v>30</v>
@@ -4603,7 +4600,7 @@
         <v>136</v>
       </c>
       <c r="Y153" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Z153">
         <v>60</v>
@@ -4614,7 +4611,7 @@
         <v>136</v>
       </c>
       <c r="Y154" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Z154">
         <v>20</v>
@@ -4625,7 +4622,7 @@
         <v>136</v>
       </c>
       <c r="Y155" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Z155">
         <v>30</v>
@@ -4636,7 +4633,7 @@
         <v>136</v>
       </c>
       <c r="Y156" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Z156">
         <v>60</v>
@@ -4647,7 +4644,7 @@
         <v>136</v>
       </c>
       <c r="Y157" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Z157">
         <v>20</v>
@@ -4658,7 +4655,7 @@
         <v>136</v>
       </c>
       <c r="Y158" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Z158">
         <v>30</v>
@@ -4669,7 +4666,7 @@
         <v>136</v>
       </c>
       <c r="Y159" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Z159">
         <v>60</v>
@@ -4677,10 +4674,10 @@
     </row>
     <row r="160" spans="24:26">
       <c r="X160" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Y160" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Z160">
         <v>20</v>
@@ -4688,10 +4685,10 @@
     </row>
     <row r="161" spans="24:26">
       <c r="X161" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Y161" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Z161">
         <v>30</v>
@@ -4699,10 +4696,10 @@
     </row>
     <row r="162" spans="24:26">
       <c r="X162" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Y162" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="Z162">
         <v>20</v>
@@ -4710,10 +4707,10 @@
     </row>
     <row r="163" spans="24:26">
       <c r="X163" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Y163" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="Z163">
         <v>30</v>
@@ -4721,10 +4718,10 @@
     </row>
     <row r="164" spans="24:26">
       <c r="X164" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Y164" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="Z164">
         <v>20</v>
@@ -4732,10 +4729,10 @@
     </row>
     <row r="165" spans="24:26">
       <c r="X165" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Y165" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="Z165">
         <v>30</v>
@@ -4743,10 +4740,10 @@
     </row>
     <row r="166" spans="24:26">
       <c r="X166" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Y166" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="Z166">
         <v>20</v>
@@ -4754,10 +4751,10 @@
     </row>
     <row r="167" spans="24:26">
       <c r="X167" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Y167" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="Z167">
         <v>30</v>
@@ -4765,10 +4762,10 @@
     </row>
     <row r="168" spans="24:26">
       <c r="X168" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Y168" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Z168">
         <v>20</v>
@@ -4776,10 +4773,10 @@
     </row>
     <row r="169" spans="24:26">
       <c r="X169" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Y169" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Z169">
         <v>30</v>
@@ -4787,10 +4784,10 @@
     </row>
     <row r="170" spans="24:26">
       <c r="X170" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Y170" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="Z170">
         <v>20</v>
@@ -4798,10 +4795,10 @@
     </row>
     <row r="171" spans="24:26">
       <c r="X171" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Y171" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="Z171">
         <v>30</v>
@@ -4809,10 +4806,10 @@
     </row>
     <row r="172" spans="24:26">
       <c r="X172" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Y172" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="Z172">
         <v>20</v>
@@ -4820,10 +4817,10 @@
     </row>
     <row r="173" spans="24:26">
       <c r="X173" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Y173" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="Z173">
         <v>30</v>
@@ -4831,10 +4828,10 @@
     </row>
     <row r="174" spans="24:26">
       <c r="X174" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Y174" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="Z174">
         <v>20</v>
@@ -4842,10 +4839,10 @@
     </row>
     <row r="175" spans="24:26">
       <c r="X175" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Y175" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="Z175">
         <v>30</v>
@@ -4853,10 +4850,10 @@
     </row>
     <row r="176" spans="24:26">
       <c r="X176" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Y176" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="Z176">
         <v>20</v>
@@ -4864,10 +4861,10 @@
     </row>
     <row r="177" spans="24:26">
       <c r="X177" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Y177" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="Z177">
         <v>30</v>
@@ -4875,10 +4872,10 @@
     </row>
     <row r="178" spans="24:26">
       <c r="X178" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Y178" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="Z178">
         <v>20</v>
@@ -4886,10 +4883,10 @@
     </row>
     <row r="179" spans="24:26">
       <c r="X179" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Y179" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="Z179">
         <v>30</v>
@@ -4897,10 +4894,10 @@
     </row>
     <row r="180" spans="24:26">
       <c r="X180" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Y180" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="Z180">
         <v>20</v>
@@ -4908,10 +4905,10 @@
     </row>
     <row r="181" spans="24:26">
       <c r="X181" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Y181" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="Z181">
         <v>30</v>
@@ -4919,10 +4916,10 @@
     </row>
     <row r="182" spans="24:26">
       <c r="X182" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Y182" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="Z182">
         <v>20</v>
@@ -4930,10 +4927,10 @@
     </row>
     <row r="183" spans="24:26">
       <c r="X183" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Y183" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="Z183">
         <v>30</v>
@@ -4941,10 +4938,10 @@
     </row>
     <row r="184" spans="24:26">
       <c r="X184" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Y184" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="Z184">
         <v>20</v>
@@ -4952,10 +4949,10 @@
     </row>
     <row r="185" spans="24:26">
       <c r="X185" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Y185" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="Z185">
         <v>30</v>
@@ -4963,10 +4960,10 @@
     </row>
     <row r="186" spans="24:26">
       <c r="X186" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Y186" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Z186">
         <v>20</v>
@@ -4974,10 +4971,10 @@
     </row>
     <row r="187" spans="24:26">
       <c r="X187" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Y187" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Z187">
         <v>30</v>
@@ -4985,10 +4982,10 @@
     </row>
     <row r="188" spans="24:26">
       <c r="X188" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Y188" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Z188">
         <v>20</v>
@@ -4996,10 +4993,10 @@
     </row>
     <row r="189" spans="24:26">
       <c r="X189" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Y189" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Z189">
         <v>30</v>
@@ -5007,10 +5004,10 @@
     </row>
     <row r="190" spans="24:26">
       <c r="X190" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Y190" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Z190">
         <v>20</v>
@@ -5018,10 +5015,10 @@
     </row>
     <row r="191" spans="24:26">
       <c r="X191" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Y191" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Z191">
         <v>30</v>
@@ -5029,10 +5026,10 @@
     </row>
     <row r="192" spans="24:26">
       <c r="X192" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Y192" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="Z192">
         <v>20</v>
@@ -5040,10 +5037,10 @@
     </row>
     <row r="193" spans="24:26">
       <c r="X193" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Y193" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="Z193">
         <v>30</v>
@@ -5051,10 +5048,10 @@
     </row>
     <row r="194" spans="24:26">
       <c r="X194" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Y194" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Z194">
         <v>20</v>
@@ -5062,10 +5059,10 @@
     </row>
     <row r="195" spans="24:26">
       <c r="X195" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Y195" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Z195">
         <v>30</v>
@@ -5073,10 +5070,10 @@
     </row>
     <row r="196" spans="24:26">
       <c r="X196" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Y196" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="Z196">
         <v>20</v>
@@ -5084,10 +5081,10 @@
     </row>
     <row r="197" spans="24:26">
       <c r="X197" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Y197" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="Z197">
         <v>30</v>
@@ -5095,10 +5092,10 @@
     </row>
     <row r="198" spans="24:26">
       <c r="X198" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Y198" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="Z198">
         <v>20</v>
@@ -5106,10 +5103,10 @@
     </row>
     <row r="199" spans="24:26">
       <c r="X199" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Y199" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="Z199">
         <v>30</v>
@@ -5117,10 +5114,10 @@
     </row>
     <row r="200" spans="24:26">
       <c r="X200" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Y200" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="Z200">
         <v>20</v>
@@ -5128,10 +5125,10 @@
     </row>
     <row r="201" spans="24:26">
       <c r="X201" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Y201" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="Z201">
         <v>30</v>
@@ -5139,10 +5136,10 @@
     </row>
     <row r="202" spans="24:26">
       <c r="X202" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Y202" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Z202">
         <v>20</v>
@@ -5150,10 +5147,10 @@
     </row>
     <row r="203" spans="24:26">
       <c r="X203" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Y203" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Z203">
         <v>30</v>
@@ -5161,10 +5158,10 @@
     </row>
     <row r="204" spans="24:26">
       <c r="X204" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Y204" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="Z204">
         <v>20</v>
@@ -5172,10 +5169,10 @@
     </row>
     <row r="205" spans="24:26">
       <c r="X205" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Y205" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="Z205">
         <v>30</v>
@@ -5183,10 +5180,10 @@
     </row>
     <row r="206" spans="24:26">
       <c r="X206" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Y206" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Z206">
         <v>20</v>
@@ -5194,10 +5191,10 @@
     </row>
     <row r="207" spans="24:26">
       <c r="X207" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Y207" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Z207">
         <v>30</v>
@@ -5205,10 +5202,10 @@
     </row>
     <row r="208" spans="24:26">
       <c r="X208" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Y208" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="Z208">
         <v>20</v>
@@ -5216,10 +5213,10 @@
     </row>
     <row r="209" spans="24:26">
       <c r="X209" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Y209" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="Z209">
         <v>30</v>
@@ -5227,10 +5224,10 @@
     </row>
     <row r="210" spans="24:26">
       <c r="X210" t="s">
+        <v>178</v>
+      </c>
+      <c r="Y210" t="s">
         <v>179</v>
-      </c>
-      <c r="Y210" t="s">
-        <v>180</v>
       </c>
       <c r="Z210">
         <v>20</v>
@@ -5238,10 +5235,10 @@
     </row>
     <row r="211" spans="24:26">
       <c r="X211" t="s">
+        <v>178</v>
+      </c>
+      <c r="Y211" t="s">
         <v>179</v>
-      </c>
-      <c r="Y211" t="s">
-        <v>180</v>
       </c>
       <c r="Z211">
         <v>30</v>
@@ -5249,10 +5246,10 @@
     </row>
     <row r="212" spans="24:26">
       <c r="X212" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Y212" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="Z212">
         <v>20</v>
@@ -5260,10 +5257,10 @@
     </row>
     <row r="213" spans="24:26">
       <c r="X213" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Y213" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="Z213">
         <v>30</v>
@@ -5526,7 +5523,7 @@
         <v>33</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C2" s="36" t="s">
         <v>34</v>
@@ -5537,7 +5534,7 @@
         <v>35</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C3" s="36" t="s">
         <v>34</v>
@@ -5780,15 +5777,15 @@
         <v>82</v>
       </c>
       <c r="Y1" s="45" t="s">
+        <v>285</v>
+      </c>
+      <c r="Z1" s="24" t="s">
         <v>286</v>
-      </c>
-      <c r="Z1" s="24" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="2" spans="1:26">
       <c r="A2" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>83</v>
@@ -5883,7 +5880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AM13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="P1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AE7" sqref="AE7"/>
     </sheetView>
   </sheetViews>
@@ -6232,19 +6229,19 @@
     </row>
     <row r="4" spans="1:39">
       <c r="A4" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="B4" s="19" t="s">
         <v>283</v>
       </c>
-      <c r="B4" s="19" t="s">
-        <v>284</v>
-      </c>
       <c r="C4" s="19" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F4" s="18">
         <v>632</v>
@@ -6562,13 +6559,13 @@
         <v>134</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E7" s="19" t="s">
         <v>136</v>
@@ -6666,16 +6663,16 @@
     </row>
     <row r="8" spans="1:39">
       <c r="A8" s="19" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E8" s="19" t="s">
         <v>136</v>
@@ -6773,16 +6770,16 @@
     </row>
     <row r="9" spans="1:39">
       <c r="A9" s="19" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E9" s="19" t="s">
         <v>136</v>
@@ -6880,16 +6877,16 @@
     </row>
     <row r="10" spans="1:39">
       <c r="A10" s="19" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E10" s="19" t="s">
         <v>136</v>
@@ -6987,16 +6984,16 @@
     </row>
     <row r="11" spans="1:39">
       <c r="A11" s="19" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E11" s="19" t="s">
         <v>136</v>
@@ -7094,16 +7091,16 @@
     </row>
     <row r="12" spans="1:39">
       <c r="A12" s="19" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E12" s="19" t="s">
         <v>136</v>
@@ -7201,16 +7198,16 @@
     </row>
     <row r="13" spans="1:39">
       <c r="A13" s="19" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E13" s="19" t="s">
         <v>136</v>
@@ -7519,136 +7516,136 @@
     </row>
     <row r="2" spans="1:3" ht="14.65" customHeight="1" thickTop="1">
       <c r="A2" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>138</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>139</v>
       </c>
       <c r="C2" s="6"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B3" s="22" t="s">
         <v>140</v>
-      </c>
-      <c r="B3" s="22" t="s">
-        <v>141</v>
       </c>
       <c r="C3" s="6"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" s="22" t="s">
         <v>142</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>143</v>
       </c>
       <c r="C4" s="6"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B5" s="22" t="s">
         <v>144</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>145</v>
       </c>
       <c r="C5" s="6"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B6" s="22" t="s">
         <v>146</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>147</v>
       </c>
       <c r="C6" s="6"/>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B7" s="22" t="s">
         <v>148</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>149</v>
       </c>
       <c r="C7" s="6"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B8" s="22" t="s">
         <v>150</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>151</v>
       </c>
       <c r="C8" s="6"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B9" s="22" t="s">
         <v>152</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>153</v>
       </c>
       <c r="C9" s="6"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B10" s="22" t="s">
         <v>154</v>
-      </c>
-      <c r="B10" s="22" t="s">
-        <v>155</v>
       </c>
       <c r="C10" s="6"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B11" s="22" t="s">
         <v>156</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>157</v>
       </c>
       <c r="C11" s="6"/>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B12" s="22" t="s">
         <v>158</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>159</v>
       </c>
       <c r="C12" s="6"/>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B13" s="22" t="s">
         <v>160</v>
-      </c>
-      <c r="B13" s="22" t="s">
-        <v>161</v>
       </c>
       <c r="C13" s="6"/>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B14" s="22" t="s">
         <v>162</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>163</v>
       </c>
       <c r="C14" s="6"/>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B15" s="22" t="s">
         <v>164</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>165</v>
       </c>
       <c r="C15" s="6"/>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B16" s="22" t="s">
         <v>166</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>167</v>
       </c>
       <c r="C16" s="6"/>
     </row>
@@ -7666,7 +7663,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -7689,7 +7686,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="14.65" customHeight="1" thickBot="1">
       <c r="A1" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B1" s="20" t="s">
         <v>84</v>
@@ -7707,25 +7704,25 @@
         <v>88</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>172</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>61</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>173</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -7748,19 +7745,19 @@
         <v>121</v>
       </c>
       <c r="G2" s="31" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H2" s="31" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I2" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="J2" s="31">
+        <v>30</v>
+      </c>
+      <c r="K2" s="31" t="s">
         <v>177</v>
-      </c>
-      <c r="J2" s="31">
-        <v>30</v>
-      </c>
-      <c r="K2" s="31" t="s">
-        <v>178</v>
       </c>
       <c r="L2" s="31">
         <v>2025</v>
@@ -7789,19 +7786,19 @@
         <v>126</v>
       </c>
       <c r="G3" s="31" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H3" s="31" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I3" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="J3" s="31">
+        <v>30</v>
+      </c>
+      <c r="K3" s="31" t="s">
         <v>177</v>
-      </c>
-      <c r="J3" s="31">
-        <v>30</v>
-      </c>
-      <c r="K3" s="31" t="s">
-        <v>178</v>
       </c>
       <c r="L3" s="31">
         <v>2025</v>
@@ -7815,34 +7812,34 @@
         <v>83</v>
       </c>
       <c r="B4" s="30" t="s">
+        <v>282</v>
+      </c>
+      <c r="C4" s="30" t="s">
         <v>283</v>
       </c>
-      <c r="C4" s="30" t="s">
-        <v>284</v>
-      </c>
       <c r="D4" s="30" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E4" s="30" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F4" s="30" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G4" s="31" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H4" s="31" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I4" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="J4" s="31">
+        <v>30</v>
+      </c>
+      <c r="K4" s="31" t="s">
         <v>177</v>
-      </c>
-      <c r="J4" s="31">
-        <v>30</v>
-      </c>
-      <c r="K4" s="31" t="s">
-        <v>178</v>
       </c>
       <c r="L4" s="31">
         <v>2025</v>
@@ -7871,19 +7868,19 @@
         <v>130</v>
       </c>
       <c r="G5" s="31" t="s">
+        <v>180</v>
+      </c>
+      <c r="H5" s="31" t="s">
         <v>181</v>
       </c>
-      <c r="H5" s="31" t="s">
-        <v>182</v>
-      </c>
       <c r="I5" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="J5" s="31">
+        <v>30</v>
+      </c>
+      <c r="K5" s="31" t="s">
         <v>177</v>
-      </c>
-      <c r="J5" s="31">
-        <v>30</v>
-      </c>
-      <c r="K5" s="31" t="s">
-        <v>178</v>
       </c>
       <c r="L5" s="31">
         <v>2025</v>
@@ -7912,19 +7909,19 @@
         <v>130</v>
       </c>
       <c r="G6" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H6" s="31" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I6" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="J6" s="31">
+        <v>30</v>
+      </c>
+      <c r="K6" s="31" t="s">
         <v>177</v>
-      </c>
-      <c r="J6" s="31">
-        <v>30</v>
-      </c>
-      <c r="K6" s="31" t="s">
-        <v>178</v>
       </c>
       <c r="L6" s="31">
         <v>2025</v>
@@ -7947,7 +7944,7 @@
         <v>136</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>137</v>
+        <v>308</v>
       </c>
       <c r="F7" s="30" t="s">
         <v>136</v>
@@ -7956,16 +7953,16 @@
         <v>136</v>
       </c>
       <c r="H7" s="31" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I7" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="J7" s="31">
+        <v>30</v>
+      </c>
+      <c r="K7" s="31" t="s">
         <v>177</v>
-      </c>
-      <c r="J7" s="31">
-        <v>30</v>
-      </c>
-      <c r="K7" s="31" t="s">
-        <v>178</v>
       </c>
       <c r="L7" s="31">
         <v>2025</v>
@@ -7979,7 +7976,7 @@
         <v>83</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C8" s="30" t="s">
         <v>135</v>
@@ -7988,7 +7985,7 @@
         <v>136</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F8" s="30" t="s">
         <v>136</v>
@@ -7997,16 +7994,16 @@
         <v>136</v>
       </c>
       <c r="H8" s="31" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I8" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="J8" s="31">
+        <v>30</v>
+      </c>
+      <c r="K8" s="31" t="s">
         <v>177</v>
-      </c>
-      <c r="J8" s="31">
-        <v>30</v>
-      </c>
-      <c r="K8" s="31" t="s">
-        <v>178</v>
       </c>
       <c r="L8" s="31">
         <v>2025</v>
@@ -8020,7 +8017,7 @@
         <v>83</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C9" s="30" t="s">
         <v>135</v>
@@ -8029,7 +8026,7 @@
         <v>136</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F9" s="30" t="s">
         <v>136</v>
@@ -8038,16 +8035,16 @@
         <v>136</v>
       </c>
       <c r="H9" s="31" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I9" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="J9" s="31">
+        <v>30</v>
+      </c>
+      <c r="K9" s="31" t="s">
         <v>177</v>
-      </c>
-      <c r="J9" s="31">
-        <v>30</v>
-      </c>
-      <c r="K9" s="31" t="s">
-        <v>178</v>
       </c>
       <c r="L9" s="31">
         <v>2025</v>
@@ -8061,7 +8058,7 @@
         <v>83</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C10" s="30" t="s">
         <v>135</v>
@@ -8070,7 +8067,7 @@
         <v>136</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F10" s="30" t="s">
         <v>136</v>
@@ -8079,16 +8076,16 @@
         <v>136</v>
       </c>
       <c r="H10" s="31" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I10" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="J10" s="31">
+        <v>30</v>
+      </c>
+      <c r="K10" s="31" t="s">
         <v>177</v>
-      </c>
-      <c r="J10" s="31">
-        <v>30</v>
-      </c>
-      <c r="K10" s="31" t="s">
-        <v>178</v>
       </c>
       <c r="L10" s="31">
         <v>2025</v>
@@ -8102,7 +8099,7 @@
         <v>83</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C11" s="30" t="s">
         <v>135</v>
@@ -8111,7 +8108,7 @@
         <v>136</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F11" s="30" t="s">
         <v>136</v>
@@ -8120,16 +8117,16 @@
         <v>136</v>
       </c>
       <c r="H11" s="31" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I11" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="J11" s="31">
+        <v>30</v>
+      </c>
+      <c r="K11" s="31" t="s">
         <v>177</v>
-      </c>
-      <c r="J11" s="31">
-        <v>30</v>
-      </c>
-      <c r="K11" s="31" t="s">
-        <v>178</v>
       </c>
       <c r="L11" s="31">
         <v>2025</v>
@@ -8143,7 +8140,7 @@
         <v>83</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C12" s="30" t="s">
         <v>135</v>
@@ -8152,7 +8149,7 @@
         <v>136</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F12" s="30" t="s">
         <v>136</v>
@@ -8161,16 +8158,16 @@
         <v>136</v>
       </c>
       <c r="H12" s="31" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I12" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="J12" s="31">
+        <v>30</v>
+      </c>
+      <c r="K12" s="31" t="s">
         <v>177</v>
-      </c>
-      <c r="J12" s="31">
-        <v>30</v>
-      </c>
-      <c r="K12" s="31" t="s">
-        <v>178</v>
       </c>
       <c r="L12" s="31">
         <v>2025</v>
@@ -8184,7 +8181,7 @@
         <v>83</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C13" s="30" t="s">
         <v>135</v>
@@ -8193,7 +8190,7 @@
         <v>136</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F13" s="30" t="s">
         <v>136</v>
@@ -8202,16 +8199,16 @@
         <v>136</v>
       </c>
       <c r="H13" s="31" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I13" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="J13" s="31">
+        <v>30</v>
+      </c>
+      <c r="K13" s="31" t="s">
         <v>177</v>
-      </c>
-      <c r="J13" s="31">
-        <v>30</v>
-      </c>
-      <c r="K13" s="31" t="s">
-        <v>178</v>
       </c>
       <c r="L13" s="31">
         <v>2025</v>
@@ -8264,134 +8261,134 @@
     </row>
     <row r="2" spans="1:3" ht="14.65" customHeight="1" thickTop="1">
       <c r="A2" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>186</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B3" s="8" t="b">
         <v>1</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B4" s="8" t="b">
         <v>1</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="B5" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>192</v>
-      </c>
-      <c r="B5" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B6" s="13">
         <v>3</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B7" s="8" t="b">
         <v>1</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="B8" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>198</v>
-      </c>
-      <c r="B8" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B9" s="8" t="b">
         <v>1</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B10" s="8" t="b">
         <v>0</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B11" s="8" t="b">
         <v>1</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B12" s="8" t="b">
         <v>0</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B13" s="8" t="b">
         <v>0</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixing issue with incorrect system portfolio file target (IL_C2N vs IL)
</commit_message>
<xml_diff>
--- a/inputs/ALEAF_inputs/ALEAF_Master_LC_GEP_IL_C2N.xlsx
+++ b/inputs/ALEAF_inputs/ALEAF_Master_LC_GEP_IL_C2N.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\biegelk\abce\inputs\ALEAF_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BBE6E58-BF75-44D7-B49B-21978B0ECD51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62CFCCFB-A59C-4BE6-BF17-97558960AC3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" tabRatio="927" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" tabRatio="927" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LC_GEP Setting" sheetId="1" r:id="rId1"/>
@@ -969,9 +969,6 @@
     <t>C2N3</t>
   </si>
   <si>
-    <t>ALEAF_IL_C2N</t>
-  </si>
-  <si>
     <t>Nuclear1</t>
   </si>
   <si>
@@ -1003,6 +1000,9 @@
   </si>
   <si>
     <t>AdvancedNuclear</t>
+  </si>
+  <si>
+    <t>ALEAF_IL</t>
   </si>
 </sst>
 </file>
@@ -1412,36 +1412,6 @@
   </cellStyles>
   <dxfs count="33">
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="left" vertical="bottom" indent="1"/>
     </dxf>
     <dxf>
@@ -1832,6 +1802,36 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1846,22 +1846,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table15" displayName="Table15" ref="A1:M14" totalsRowShown="0" dataDxfId="18" headerRowBorderDxfId="19" headerRowCellStyle="Heading 3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table15" displayName="Table15" ref="A1:M14" totalsRowShown="0" dataDxfId="15" headerRowBorderDxfId="16" headerRowCellStyle="Heading 3">
   <autoFilter ref="A1:M14" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ATB_Setting_ID" dataDxfId="17" dataCellStyle="20% - Accent4"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tech_ID" dataDxfId="16" dataCellStyle="20% - Accent4"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="UNITGROUP" dataDxfId="15" dataCellStyle="20% - Accent4"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="UNIT_CATEGORY" dataDxfId="14" dataCellStyle="20% - Accent4"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="UNIT_TYPE" dataDxfId="13" dataCellStyle="20% - Accent4"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="FUEL" dataDxfId="12" dataCellStyle="20% - Accent4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Tech" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="TechDetail" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Case" dataDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="CRP" dataDxfId="8"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Scenario" dataDxfId="7"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Year" dataDxfId="6"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="ATB Year" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ATB_Setting_ID" dataDxfId="14" dataCellStyle="20% - Accent4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tech_ID" dataDxfId="13" dataCellStyle="20% - Accent4"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="UNITGROUP" dataDxfId="12" dataCellStyle="20% - Accent4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="UNIT_CATEGORY" dataDxfId="11" dataCellStyle="20% - Accent4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="UNIT_TYPE" dataDxfId="10" dataCellStyle="20% - Accent4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="FUEL" dataDxfId="9" dataCellStyle="20% - Accent4"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Tech" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="TechDetail" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Case" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="CRP" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Scenario" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Year" dataDxfId="3"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="ATB Year" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1950,10 +1950,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table2" displayName="Table2" ref="I1:I6" totalsRowShown="0" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table2" displayName="Table2" ref="I1:I6" totalsRowShown="0" dataDxfId="1">
   <autoFilter ref="I1:I6" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Battery" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Battery" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5538,7 +5538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -5576,7 +5576,7 @@
         <v>35</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>299</v>
+        <v>310</v>
       </c>
       <c r="C3" s="36" t="s">
         <v>34</v>
@@ -5922,8 +5922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AM14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V14" sqref="V14"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -6601,13 +6601,13 @@
         <v>134</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E7" s="19" t="s">
         <v>135</v>
@@ -6708,10 +6708,10 @@
         <v>287</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D8" s="19" t="s">
         <v>293</v>
@@ -6815,10 +6815,10 @@
         <v>288</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D9" s="19" t="s">
         <v>294</v>
@@ -6922,10 +6922,10 @@
         <v>289</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D10" s="19" t="s">
         <v>295</v>
@@ -7029,10 +7029,10 @@
         <v>290</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D11" s="19" t="s">
         <v>296</v>
@@ -7136,10 +7136,10 @@
         <v>291</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D12" s="19" t="s">
         <v>297</v>
@@ -7243,10 +7243,10 @@
         <v>292</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D13" s="19" t="s">
         <v>298</v>
@@ -7347,16 +7347,16 @@
     </row>
     <row r="14" spans="1:39">
       <c r="A14" s="19" t="s">
+        <v>307</v>
+      </c>
+      <c r="B14" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="C14" s="19" t="s">
+        <v>308</v>
+      </c>
+      <c r="D14" s="19" t="s">
         <v>309</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>309</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>310</v>
       </c>
       <c r="E14" s="19" t="s">
         <v>135</v>
@@ -7634,7 +7634,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH14">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
     <cfRule type="colorScale" priority="2">
@@ -7649,7 +7649,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI14">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
     <cfRule type="colorScale" priority="4">
@@ -7664,7 +7664,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD14:AF14">
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="5" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
     <cfRule type="colorScale" priority="6">
@@ -8132,13 +8132,13 @@
         <v>134</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F7" s="30" t="s">
         <v>135</v>
@@ -8173,10 +8173,10 @@
         <v>287</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E8" s="19" t="s">
         <v>293</v>
@@ -8214,10 +8214,10 @@
         <v>288</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E9" s="19" t="s">
         <v>294</v>
@@ -8255,10 +8255,10 @@
         <v>289</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E10" s="19" t="s">
         <v>295</v>
@@ -8296,10 +8296,10 @@
         <v>290</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E11" s="19" t="s">
         <v>296</v>
@@ -8337,10 +8337,10 @@
         <v>291</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E12" s="19" t="s">
         <v>297</v>
@@ -8378,10 +8378,10 @@
         <v>292</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E13" s="19" t="s">
         <v>298</v>
@@ -8416,16 +8416,16 @@
         <v>83</v>
       </c>
       <c r="B14" s="30" t="s">
+        <v>307</v>
+      </c>
+      <c r="C14" s="30" t="s">
         <v>308</v>
       </c>
-      <c r="C14" s="30" t="s">
+      <c r="D14" s="30" t="s">
+        <v>308</v>
+      </c>
+      <c r="E14" s="30" t="s">
         <v>309</v>
-      </c>
-      <c r="D14" s="30" t="s">
-        <v>309</v>
-      </c>
-      <c r="E14" s="30" t="s">
-        <v>310</v>
       </c>
       <c r="F14" s="30" t="s">
         <v>135</v>

</xml_diff>

<commit_message>
temporary data updates for testing
</commit_message>
<xml_diff>
--- a/inputs/ALEAF_inputs/ALEAF_Master_LC_GEP_IL_C2N.xlsx
+++ b/inputs/ALEAF_inputs/ALEAF_Master_LC_GEP_IL_C2N.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\biegelk\abce\inputs\ALEAF_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62CFCCFB-A59C-4BE6-BF17-97558960AC3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F31A42-841A-4181-AE94-34B17F503268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" tabRatio="927" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" tabRatio="927" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LC_GEP Setting" sheetId="1" r:id="rId1"/>
@@ -5538,7 +5538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -5922,8 +5922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AM14"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -6839,7 +6839,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="18">
-        <v>3464</v>
+        <v>3598</v>
       </c>
       <c r="K9" s="18">
         <v>5.1999999999999998E-2</v>
@@ -7053,7 +7053,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="18">
-        <v>3546</v>
+        <v>3951</v>
       </c>
       <c r="K11" s="18">
         <v>5.1999999999999998E-2</v>
@@ -7267,7 +7267,7 @@
         <v>0</v>
       </c>
       <c r="J13" s="18">
-        <v>3318</v>
+        <v>1000</v>
       </c>
       <c r="K13" s="18">
         <v>5.1999999999999998E-2</v>
@@ -7276,7 +7276,7 @@
         <v>0</v>
       </c>
       <c r="M13" s="18">
-        <v>105.17</v>
+        <v>10</v>
       </c>
       <c r="N13" s="18">
         <v>2</v>

</xml_diff>